<commit_message>
added empties to notebook to be filled
</commit_message>
<xml_diff>
--- a/WrittenLanguageDataTypes.xlsx
+++ b/WrittenLanguageDataTypes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karso\Desktop\PromptRecovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A01A54-F3FE-46CC-AC95-1E546BD26A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8772C76-641C-474B-9E59-2ACA6E017E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9168" yWindow="2064" windowWidth="12528" windowHeight="8880" xr2:uid="{3893CAB6-0FBF-4A73-858A-C7DF6F6B8EC1}"/>
+    <workbookView xWindow="9168" yWindow="0" windowWidth="12528" windowHeight="12336" xr2:uid="{3893CAB6-0FBF-4A73-858A-C7DF6F6B8EC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data_Types" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="79">
   <si>
     <t>WikiTV2023.csv</t>
   </si>
@@ -258,6 +258,21 @@
   </si>
   <si>
     <t>email_msgs_clean.csv</t>
+  </si>
+  <si>
+    <t>Interview Questions</t>
+  </si>
+  <si>
+    <t>Song Lyrics</t>
+  </si>
+  <si>
+    <t>Poems</t>
+  </si>
+  <si>
+    <t>Maxims</t>
+  </si>
+  <si>
+    <t>Quotes</t>
   </si>
 </sst>
 </file>
@@ -722,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{192A6510-5D95-4AEA-8FBF-55B25D9B825C}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -770,83 +785,63 @@
         <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="3">
-        <v>13734</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="3">
-        <v>74</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F4" s="3">
-        <v>30</v>
+        <v>13734</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>30</v>
@@ -855,16 +850,16 @@
         <v>35</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="F5" s="3">
+        <v>74</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -872,7 +867,7 @@
         <v>24</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>31</v>
@@ -881,16 +876,16 @@
         <v>35</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F6" s="3">
-        <v>91</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -898,111 +893,111 @@
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="3">
-        <v>3898</v>
+        <v>66</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>46</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="F8" s="3">
+        <v>91</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>39</v>
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="F9" s="3">
-        <v>6000</v>
+        <v>3898</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>15</v>
+      <c r="H9" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1380</v>
+        <v>37</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>59</v>
+      <c r="H10" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>30</v>
@@ -1011,76 +1006,66 @@
         <v>35</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F11" s="3">
-        <v>153</v>
+        <v>6000</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="F12" s="3">
-        <v>2208</v>
+        <v>1380</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>55</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="3">
-        <v>300</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>30</v>
@@ -1089,110 +1074,117 @@
         <v>35</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14" s="3">
-        <v>2717</v>
+        <v>153</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2208</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="F16" s="3">
+        <v>300</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="1"/>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F17" s="3">
+        <v>2717</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>62</v>
-      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>77</v>
+      </c>
       <c r="C19" s="1" t="s">
         <v>30</v>
       </c>
@@ -1203,53 +1195,156 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
+      <c r="D20" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="C21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
+      <c r="D21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F23">
-        <f>SUM(F2:F22)</f>
+      <c r="A23" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F28">
+        <f>SUM(F4:F27)</f>
         <v>30585</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H22">
-    <sortCondition descending="1" ref="A1:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:H27">
+    <sortCondition descending="1" ref="A1:A27"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:D1048576">
+  <conditionalFormatting sqref="A2:A3 A4:D1048576">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
       <formula>"Misc"</formula>
     </cfRule>
@@ -1273,8 +1368,8 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="H9" r:id="rId1" display="https://github.com/rowanz/hellaswag/blob/master/data/hellaswag_train.jsonl" xr:uid="{1B644A2B-414C-4D74-B239-5052551623BE}"/>
-    <hyperlink ref="H8" r:id="rId2" xr:uid="{453E49A5-1D9F-4C15-AB1F-E50584FEAE35}"/>
+    <hyperlink ref="H11" r:id="rId1" display="https://github.com/rowanz/hellaswag/blob/master/data/hellaswag_train.jsonl" xr:uid="{1B644A2B-414C-4D74-B239-5052551623BE}"/>
+    <hyperlink ref="H10" r:id="rId2" xr:uid="{453E49A5-1D9F-4C15-AB1F-E50584FEAE35}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>